<commit_message>
add module lookup & resources & webservices test ui & register & international
</commit_message>
<xml_diff>
--- a/documents/designer/功能进度计划.xlsx
+++ b/documents/designer/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>需求名称</t>
   </si>
@@ -80,6 +80,172 @@
   </si>
   <si>
     <t>待前置步骤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">icustom.core filter </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公共静态资源加载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成</t>
+  </si>
+  <si>
+    <t>完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限springboot 组件自动加载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜单管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有的资源为何请求报200,应该报404</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂停</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加急优先</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0066"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>加</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>急</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>优</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>先</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待续</t>
+  </si>
+  <si>
+    <t>开发数据字典</t>
+  </si>
+  <si>
+    <t>功能维度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>security 4 testing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORACLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CORE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SECURITY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MENU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rest webservices 测试UI界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件上传下载组件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入导出excel组件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动化测试selenium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加文件请求时的时间戳过滤器,每次能加载最新的,主要是CSS和JS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按数据字典状态和code查询,给时间戳增加启用状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国际化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写一个页面JS分页插件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发邮件功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发BBS功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发工作流，并且有demo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+/services/sys/resourcesService/findResourcesSiteMenu没有开发路径应该是404
+加请求头验证
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -87,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +284,54 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0066"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,7 +355,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -159,12 +373,42 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -190,24 +434,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="微软雅黑"/>
-        <scheme val="none"/>
-      </font>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -341,6 +567,7 @@
         <name val="微软雅黑"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -359,24 +586,47 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="0" hidden="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0066"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:I2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I20"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="序列" dataDxfId="10"/>
-    <tableColumn id="2" name="需求名称" dataDxfId="9"/>
-    <tableColumn id="3" name="优先级别" dataDxfId="8"/>
-    <tableColumn id="4" name="完成状态" dataDxfId="7"/>
-    <tableColumn id="5" name="计划类型" dataDxfId="6"/>
-    <tableColumn id="6" name="状态" dataDxfId="5"/>
-    <tableColumn id="7" name="计划日期" dataDxfId="4"/>
-    <tableColumn id="8" name="完成日期" dataDxfId="3"/>
-    <tableColumn id="9" name="补充说明" dataDxfId="2"/>
+    <tableColumn id="1" name="序列" dataDxfId="8"/>
+    <tableColumn id="2" name="需求名称" dataDxfId="7"/>
+    <tableColumn id="3" name="优先级别" dataDxfId="6"/>
+    <tableColumn id="4" name="完成状态" dataDxfId="5"/>
+    <tableColumn id="5" name="计划类型" dataDxfId="4"/>
+    <tableColumn id="6" name="功能维度" dataDxfId="3"/>
+    <tableColumn id="7" name="计划日期" dataDxfId="2"/>
+    <tableColumn id="8" name="完成日期" dataDxfId="1"/>
+    <tableColumn id="9" name="补充说明" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -667,20 +917,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="26.625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1"/>
-    <col min="7" max="9" width="10.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="15"/>
+    <col min="2" max="2" width="41.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="13.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="53.875" style="1" customWidth="1"/>
     <col min="10" max="13" width="9" style="1"/>
     <col min="14" max="14" width="15.625" style="1" customWidth="1"/>
     <col min="15" max="15" width="11.25" style="1" bestFit="1" customWidth="1"/>
@@ -688,7 +941,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -704,7 +957,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -717,11 +970,19 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A2" s="2"/>
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
@@ -730,18 +991,52 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="24.75" customHeight="1">
-      <c r="L3" s="1" t="s">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="5">
         <v>42879</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="24.75" customHeight="1">
-      <c r="L4" s="1" t="s">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="L4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -749,6 +1044,23 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="L5" s="1" t="s">
         <v>14</v>
       </c>
@@ -757,23 +1069,272 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="24.75" customHeight="1">
-      <c r="L6" s="1" t="s">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="L6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.75" customHeight="1">
-      <c r="L7" s="1" t="s">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="10" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="8" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="L8" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="L10" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="L11" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A12" s="14">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A13" s="14">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A14" s="14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A15" s="14">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="24.75" customHeight="1">
+      <c r="A16" s="14">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A17" s="14">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A18" s="14">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A19" s="14">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A20" s="14">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
-      <formula1>$L$3:$L$7</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20">
+      <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
-      <formula1>$N$3:$N$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>$L$3:$L$11</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add module sso develop lookup and register and international
</commit_message>
<xml_diff>
--- a/documents/designer/功能进度计划.xlsx
+++ b/documents/designer/功能进度计划.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>需求名称</t>
   </si>
@@ -248,12 +248,27 @@
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>icustom.sso</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>补齐数据模型和设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>补齐api文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂停</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +347,14 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -355,7 +378,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -409,6 +432,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,8 +641,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I23" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I23"/>
   <tableColumns count="9">
     <tableColumn id="1" name="序列" dataDxfId="8"/>
     <tableColumn id="2" name="需求名称" dataDxfId="7"/>
@@ -917,11 +943,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1"/>
@@ -1094,11 +1120,11 @@
       <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="2"/>
@@ -1200,7 +1226,9 @@
         <v>39</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1215,7 +1243,9 @@
         <v>40</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1230,7 +1260,9 @@
         <v>41</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1245,7 +1277,9 @@
         <v>42</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1260,7 +1294,9 @@
         <v>43</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1275,7 +1311,9 @@
         <v>44</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1290,7 +1328,9 @@
         <v>45</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1305,7 +1345,9 @@
         <v>46</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1320,17 +1362,70 @@
         <v>47</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
+    <row r="21" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A21" s="14">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A22" s="14">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" ht="24.75" customHeight="1">
+      <c r="A23" s="14">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">

</xml_diff>